<commit_message>
PROS-4783 - CCRU - CCH Integration - Debugging
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/HoReCa Restaurant_Cafe PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/HoReCa Restaurant_Cafe PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="HoReCa Restaurant_Cafe" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,6 +38,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$B$1:$AS$46</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$B$1:$AS$46</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$B$1:$AS$46</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$B$1:$AS$46</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -146,7 +147,7 @@
     <t xml:space="preserve">SAP KPI</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI CCH ID</t>
+    <t xml:space="preserve">CCH KPI ID</t>
   </si>
   <si>
     <t xml:space="preserve">KPI name Eng</t>
@@ -1588,9 +1589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1787760</xdr:colOff>
+      <xdr:colOff>1787400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1600,7 +1601,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="18997560" cy="10164960"/>
+          <a:ext cx="19501920" cy="10164600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1633,9 +1634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1787760</xdr:colOff>
+      <xdr:colOff>1787400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1645,7 +1646,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="18997560" cy="10164960"/>
+          <a:ext cx="19501920" cy="10164600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1678,9 +1679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1787760</xdr:colOff>
+      <xdr:colOff>1787400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1690,7 +1691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="18997560" cy="10164960"/>
+          <a:ext cx="19501920" cy="10164600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1723,9 +1724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1787760</xdr:colOff>
+      <xdr:colOff>1787400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1735,7 +1736,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="18997560" cy="10164960"/>
+          <a:ext cx="19501920" cy="10164600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1768,9 +1769,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1787760</xdr:colOff>
+      <xdr:colOff>1787400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1780,7 +1781,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="18997560" cy="10164960"/>
+          <a:ext cx="19501920" cy="10164600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1815,48 +1816,48 @@
   </sheetPr>
   <dimension ref="A1:AS55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R48" activeCellId="0" sqref="R48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="32.1209302325581"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="65.2232558139535"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="1" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="22" min="19" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="1" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="30" min="28" style="1" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="4" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="3" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="5" width="59.3162790697674"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="5" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="5" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="33.1023255813953"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="67.1906976744186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="1" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="22" min="19" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="1" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="1" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="4" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="3" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="5" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="5" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="5" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,6 +4176,7 @@
       <c r="I27" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="J27" s="0"/>
       <c r="K27" s="72" t="n">
         <v>2</v>
       </c>
@@ -5602,6 +5604,7 @@
       <c r="I43" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="J43" s="0"/>
       <c r="K43" s="77" t="n">
         <v>1</v>
       </c>
@@ -5686,6 +5689,7 @@
       <c r="I44" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="J44" s="0"/>
       <c r="K44" s="39" t="n">
         <v>1</v>
       </c>
@@ -6640,7 +6644,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>